<commit_message>
Changed this, that, and the other thing
</commit_message>
<xml_diff>
--- a/src/Batteries.xlsx
+++ b/src/Batteries.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Himanshu\OneDrive - Prevalon Energy\I drive\Sizing Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://prevalonenergy-my.sharepoint.com/personal/himanshu_prevalonenergy_com/Documents/I drive/Sizing Tool/DeployWithRender/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EA821F-A641-4A2D-81A0-B6347A03F243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{A3EA821F-A641-4A2D-81A0-B6347A03F243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C48DE0D-7073-4BA0-9A9C-FFE16AE44CA7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Model</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>HD 511</t>
+  </si>
+  <si>
+    <t>usable_capacity_ratio_at_0.3333333333333333C</t>
+  </si>
+  <si>
+    <t>usable_capacity_ratio_at_0.16666666666666666C</t>
+  </si>
+  <si>
+    <t>usable_capacity_ratio_at_0.125C</t>
   </si>
 </sst>
 </file>
@@ -115,7 +124,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -164,7 +173,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,15 +454,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -717,59 +726,101 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.92</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.93</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B19" s="5">
         <v>0.94</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C19" s="5">
         <v>0.95</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D19" s="5">
         <f>D17</f>
         <v>0.97</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="C19" s="5">
-        <v>0.96</v>
-      </c>
-      <c r="D19" s="5">
-        <f>D18</f>
-        <v>0.97</v>
-      </c>
-    </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1">
-        <v>18</v>
-      </c>
-      <c r="C20" s="1">
-        <v>18</v>
-      </c>
-      <c r="D20" s="1">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.96</v>
+      </c>
+      <c r="D20" s="5">
+        <f>D19</f>
+        <v>0.97</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.96</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0.96</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>18</v>
+      </c>
+      <c r="C23" s="1">
+        <v>18</v>
+      </c>
+      <c r="D23" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B24" s="6">
         <v>35</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C24" s="6">
         <v>44</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D24" s="1">
         <v>52</v>
       </c>
     </row>

</xml_diff>